<commit_message>
Working version of branch and price with L-shaped subproblems
</commit_message>
<xml_diff>
--- a/output/instance_SMALL_scenario_2/column_variable_values_site0_iteration1.xlsx
+++ b/output/instance_SMALL_scenario_2/column_variable_values_site0_iteration1.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,16 +524,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E2" t="n">
-        <v>95429.78</v>
+        <v>90564.17</v>
       </c>
       <c r="F2" t="n">
-        <v>95429.78</v>
+        <v>90564.17</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -559,13 +559,13 @@
       <c r="B3" s="1" t="n"/>
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>154639.84</v>
+        <v>147741.33</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -591,13 +591,13 @@
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>223631.39</v>
+        <v>257117.05</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -623,13 +623,13 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>326229.78</v>
+        <v>517179.5</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -655,13 +655,13 @@
       <c r="B6" s="1" t="n"/>
       <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>435665.85</v>
+        <v>856511.16</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -687,13 +687,13 @@
       <c r="B7" s="1" t="n"/>
       <c r="C7" s="1" t="n"/>
       <c r="D7" s="1" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>529891.23</v>
+        <v>1208501.9</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -719,13 +719,13 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>580974.5600000001</v>
+        <v>1433065.24</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -751,13 +751,13 @@
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n"/>
       <c r="D9" s="1" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>642457.36</v>
+        <v>1613513.76</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -783,13 +783,13 @@
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n"/>
       <c r="D10" s="1" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>758977.63</v>
+        <v>1790023.1</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>938656.3100000001</v>
+        <v>1915683.94</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -847,13 +847,13 @@
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="1" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1289368.97</v>
+        <v>2044148.98</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -879,13 +879,13 @@
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1694412.08</v>
+        <v>2190582.98</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>2104248.55</v>
+        <v>2438726.25</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -943,16 +943,16 @@
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="n"/>
       <c r="D15" s="1" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>2499043.27</v>
+        <v>2871658.48</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -975,16 +975,16 @@
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="n"/>
       <c r="D16" s="1" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>2873394.69</v>
+        <v>2514032.61</v>
       </c>
       <c r="G16" t="n">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="17">
@@ -1007,16 +1007,16 @@
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>2193899.28</v>
+        <v>3072715.81</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>3618984.24</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1031,30 +1031,32 @@
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
+      <c r="C18" s="1" t="n">
+        <v>41</v>
+      </c>
       <c r="D18" s="1" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>98378.85000000001</v>
       </c>
       <c r="F18" t="n">
-        <v>2391072.27</v>
+        <v>98378.85000000001</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
@@ -1071,13 +1073,13 @@
       <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="n"/>
       <c r="D19" s="1" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>2547264.6</v>
+        <v>121499.34</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1103,13 +1105,13 @@
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>2668833.72</v>
+        <v>168897.57</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -1135,13 +1137,13 @@
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="n"/>
       <c r="D21" s="1" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>2829398.18</v>
+        <v>308470.91</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1159,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1167,16 +1169,16 @@
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="n"/>
       <c r="D22" s="1" t="n">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>3101680.14</v>
+        <v>578236.84</v>
       </c>
       <c r="G22" t="n">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1191,7 +1193,7 @@
         <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1199,13 +1201,13 @@
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="1" t="n">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>2549989.13</v>
+        <v>1004491.05</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1223,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1231,16 +1233,16 @@
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="n"/>
       <c r="D24" s="1" t="n">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>2999477.03</v>
+        <v>1321104.27</v>
       </c>
       <c r="G24" t="n">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1255,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1263,16 +1265,16 @@
       <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="n"/>
       <c r="D25" s="1" t="n">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>2554507.7</v>
+        <v>1586656.6</v>
       </c>
       <c r="G25" t="n">
-        <v>2937412.89</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1287,32 +1289,30 @@
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="n"/>
-      <c r="C26" s="1" t="n">
-        <v>42</v>
-      </c>
+      <c r="C26" s="1" t="n"/>
       <c r="D26" s="1" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E26" t="n">
-        <v>8696.23</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>8696.23</v>
+        <v>1850518.22</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
         <v>1</v>
@@ -1329,13 +1329,13 @@
       <c r="B27" s="1" t="n"/>
       <c r="C27" s="1" t="n"/>
       <c r="D27" s="1" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>12106.9</v>
+        <v>2061249.64</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1361,13 +1361,13 @@
       <c r="B28" s="1" t="n"/>
       <c r="C28" s="1" t="n"/>
       <c r="D28" s="1" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>19361.62</v>
+        <v>2308606.84</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1393,13 +1393,13 @@
       <c r="B29" s="1" t="n"/>
       <c r="C29" s="1" t="n"/>
       <c r="D29" s="1" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>38483.39</v>
+        <v>2478782.76</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1425,13 +1425,13 @@
       <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="n"/>
       <c r="D30" s="1" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>71545.42999999999</v>
+        <v>2610944.93</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1457,13 +1457,13 @@
       <c r="B31" s="1" t="n"/>
       <c r="C31" s="1" t="n"/>
       <c r="D31" s="1" t="n">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>110767.93</v>
+        <v>2794262.03</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1489,16 +1489,16 @@
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="n"/>
       <c r="D32" s="1" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>136484.36</v>
+        <v>3119992.19</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1047799.77</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1521,13 +1521,13 @@
       <c r="B33" s="1" t="n"/>
       <c r="C33" s="1" t="n"/>
       <c r="D33" s="1" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>157635.27</v>
+        <v>2594034.49</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -1553,16 +1553,16 @@
       <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="n"/>
       <c r="D34" s="1" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>178126.69</v>
+        <v>3120000</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>1111413.86</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1585,13 +1585,13 @@
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="n"/>
       <c r="D35" s="1" t="n">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>194599.62</v>
+        <v>2667584.6</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -1617,16 +1617,16 @@
       <c r="B36" s="1" t="n"/>
       <c r="C36" s="1" t="n"/>
       <c r="D36" s="1" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>211699.06</v>
+        <v>3120000</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>3649143.88</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1641,30 +1641,36 @@
         <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="n"/>
-      <c r="C37" s="1" t="n"/>
+      <c r="A37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>19</v>
+      </c>
       <c r="D37" s="1" t="n">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>90564.17</v>
       </c>
       <c r="F37" t="n">
-        <v>223221.73</v>
+        <v>90564.17</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="n">
         <v>1</v>
@@ -1681,13 +1687,13 @@
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="n">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>238377.54</v>
+        <v>150491.55</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -1713,13 +1719,13 @@
       <c r="B39" s="1" t="n"/>
       <c r="C39" s="1" t="n"/>
       <c r="D39" s="1" t="n">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>265416.65</v>
+        <v>266507.96</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -1745,13 +1751,13 @@
       <c r="B40" s="1" t="n"/>
       <c r="C40" s="1" t="n"/>
       <c r="D40" s="1" t="n">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>312332.97</v>
+        <v>545655.9300000001</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -1777,13 +1783,13 @@
       <c r="B41" s="1" t="n"/>
       <c r="C41" s="1" t="n"/>
       <c r="D41" s="1" t="n">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>376396.33</v>
+        <v>913132.04</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -1809,13 +1815,13 @@
       <c r="B42" s="1" t="n"/>
       <c r="C42" s="1" t="n"/>
       <c r="D42" s="1" t="n">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>456765.68</v>
+        <v>1296347.39</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
@@ -1841,13 +1847,13 @@
       <c r="B43" s="1" t="n"/>
       <c r="C43" s="1" t="n"/>
       <c r="D43" s="1" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>535017.11</v>
+        <v>1541554.13</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -1869,32 +1875,26 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A44" s="1" t="n"/>
+      <c r="B44" s="1" t="n"/>
+      <c r="C44" s="1" t="n"/>
       <c r="D44" s="1" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E44" t="n">
-        <v>95429.78</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>95429.78</v>
+        <v>1738907.83</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
         <v>1</v>
@@ -1911,13 +1911,13 @@
       <c r="B45" s="1" t="n"/>
       <c r="C45" s="1" t="n"/>
       <c r="D45" s="1" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>157482.13</v>
+        <v>1932179.23</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -1943,13 +1943,13 @@
       <c r="B46" s="1" t="n"/>
       <c r="C46" s="1" t="n"/>
       <c r="D46" s="1" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>230495.34</v>
+        <v>2069910.05</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -1975,13 +1975,13 @@
       <c r="B47" s="1" t="n"/>
       <c r="C47" s="1" t="n"/>
       <c r="D47" s="1" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>339898.42</v>
+        <v>2210807.47</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
@@ -2007,13 +2007,13 @@
       <c r="B48" s="1" t="n"/>
       <c r="C48" s="1" t="n"/>
       <c r="D48" s="1" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>457288.86</v>
+        <v>2371510.46</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -2039,13 +2039,13 @@
       <c r="B49" s="1" t="n"/>
       <c r="C49" s="1" t="n"/>
       <c r="D49" s="1" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>558765.47</v>
+        <v>2644017.44</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
@@ -2071,16 +2071,16 @@
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="n"/>
       <c r="D50" s="1" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>613913.38</v>
+        <v>3119987.3</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>1280356.46</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -2095,7 +2095,7 @@
         <v>1</v>
       </c>
       <c r="L50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -2103,13 +2103,13 @@
       <c r="B51" s="1" t="n"/>
       <c r="C51" s="1" t="n"/>
       <c r="D51" s="1" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>680379.8199999999</v>
+        <v>2546920.51</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -2135,16 +2135,16 @@
       <c r="B52" s="1" t="n"/>
       <c r="C52" s="1" t="n"/>
       <c r="D52" s="1" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>806563.96</v>
+        <v>3120000</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1198209.3</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2159,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="L52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2167,13 +2167,13 @@
       <c r="B53" s="1" t="n"/>
       <c r="C53" s="1" t="n"/>
       <c r="D53" s="1" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>1001629.07</v>
+        <v>2482889.48</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
@@ -2199,13 +2199,13 @@
       <c r="B54" s="1" t="n"/>
       <c r="C54" s="1" t="n"/>
       <c r="D54" s="1" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>1383611</v>
+        <v>2820621.19</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
@@ -2231,16 +2231,16 @@
       <c r="B55" s="1" t="n"/>
       <c r="C55" s="1" t="n"/>
       <c r="D55" s="1" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>1826220.44</v>
+        <v>3120000</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>3380626.21</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2255,30 +2255,32 @@
         <v>1</v>
       </c>
       <c r="L55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="n"/>
+      <c r="C56" s="1" t="n">
+        <v>41</v>
+      </c>
       <c r="D56" s="1" t="n">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>98378.85000000001</v>
       </c>
       <c r="F56" t="n">
-        <v>2275189.47</v>
+        <v>98378.85000000001</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="n">
         <v>1</v>
@@ -2295,13 +2297,13 @@
       <c r="B57" s="1" t="n"/>
       <c r="C57" s="1" t="n"/>
       <c r="D57" s="1" t="n">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>2708485.33</v>
+        <v>122522.26</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
@@ -2327,16 +2329,16 @@
       <c r="B58" s="1" t="n"/>
       <c r="C58" s="1" t="n"/>
       <c r="D58" s="1" t="n">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>3119927.51</v>
+        <v>172353.43</v>
       </c>
       <c r="G58" t="n">
-        <v>1060741.23</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2351,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2359,13 +2361,13 @@
       <c r="B59" s="1" t="n"/>
       <c r="C59" s="1" t="n"/>
       <c r="D59" s="1" t="n">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>2411833.36</v>
+        <v>320644.53</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -2391,13 +2393,13 @@
       <c r="B60" s="1" t="n"/>
       <c r="C60" s="1" t="n"/>
       <c r="D60" s="1" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>2631375.59</v>
+        <v>610494.12</v>
       </c>
       <c r="G60" t="n">
         <v>0</v>
@@ -2423,13 +2425,13 @@
       <c r="B61" s="1" t="n"/>
       <c r="C61" s="1" t="n"/>
       <c r="D61" s="1" t="n">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>2805408.67</v>
+        <v>1072460.64</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -2455,13 +2457,13 @@
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="n"/>
       <c r="D62" s="1" t="n">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>2940939.75</v>
+        <v>1417332.09</v>
       </c>
       <c r="G62" t="n">
         <v>0</v>
@@ -2487,16 +2489,16 @@
       <c r="B63" s="1" t="n"/>
       <c r="C63" s="1" t="n"/>
       <c r="D63" s="1" t="n">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>3120000</v>
+        <v>1707338.81</v>
       </c>
       <c r="G63" t="n">
-        <v>1113460.64</v>
+        <v>0</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2511,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="L63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2519,13 +2521,13 @@
       <c r="B64" s="1" t="n"/>
       <c r="C64" s="1" t="n"/>
       <c r="D64" s="1" t="n">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>2310316.63</v>
+        <v>1996018.74</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
@@ -2551,13 +2553,13 @@
       <c r="B65" s="1" t="n"/>
       <c r="C65" s="1" t="n"/>
       <c r="D65" s="1" t="n">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>2648075.33</v>
+        <v>2226890.93</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2583,16 +2585,16 @@
       <c r="B66" s="1" t="n"/>
       <c r="C66" s="1" t="n"/>
       <c r="D66" s="1" t="n">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>3120000</v>
+        <v>2498175.29</v>
       </c>
       <c r="G66" t="n">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2607,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="L66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2615,16 +2617,16 @@
       <c r="B67" s="1" t="n"/>
       <c r="C67" s="1" t="n"/>
       <c r="D67" s="1" t="n">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>2703367.11</v>
+        <v>2684998.85</v>
       </c>
       <c r="G67" t="n">
-        <v>3112553.99</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2639,32 +2641,30 @@
         <v>1</v>
       </c>
       <c r="L67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="n"/>
-      <c r="C68" s="1" t="n">
-        <v>42</v>
-      </c>
+      <c r="C68" s="1" t="n"/>
       <c r="D68" s="1" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E68" t="n">
-        <v>8696.23</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>8696.23</v>
+        <v>2830191.26</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="n">
         <v>1</v>
@@ -2681,16 +2681,16 @@
       <c r="B69" s="1" t="n"/>
       <c r="C69" s="1" t="n"/>
       <c r="D69" s="1" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>12263.27</v>
+        <v>3031666.5</v>
       </c>
       <c r="G69" t="n">
-        <v>0</v>
+        <v>1176488.5</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2705,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="L69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2713,13 +2713,13 @@
       <c r="B70" s="1" t="n"/>
       <c r="C70" s="1" t="n"/>
       <c r="D70" s="1" t="n">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>19924.6</v>
+        <v>2213399.04</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -2745,16 +2745,16 @@
       <c r="B71" s="1" t="n"/>
       <c r="C71" s="1" t="n"/>
       <c r="D71" s="1" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>40360.9</v>
+        <v>2588510.22</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2777,16 +2777,16 @@
       <c r="B72" s="1" t="n"/>
       <c r="C72" s="1" t="n"/>
       <c r="D72" s="1" t="n">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>76070.2</v>
+        <v>3120000</v>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>1123532.22</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="L72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2809,13 +2809,13 @@
       <c r="B73" s="1" t="n"/>
       <c r="C73" s="1" t="n"/>
       <c r="D73" s="1" t="n">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>118726.28</v>
+        <v>2663314.55</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
@@ -2841,16 +2841,16 @@
       <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="n"/>
       <c r="D74" s="1" t="n">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>146797.75</v>
+        <v>3120000</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>3654994.48</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2865,371 +2865,19 @@
         <v>1</v>
       </c>
       <c r="L74" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n"/>
-      <c r="B75" s="1" t="n"/>
-      <c r="C75" s="1" t="n"/>
-      <c r="D75" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="E75" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" t="n">
-        <v>169930.3</v>
-      </c>
-      <c r="G75" t="n">
-        <v>0</v>
-      </c>
-      <c r="H75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J75" t="n">
-        <v>1</v>
-      </c>
-      <c r="K75" t="n">
-        <v>1</v>
-      </c>
-      <c r="L75" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="n"/>
-      <c r="C76" s="1" t="n"/>
-      <c r="D76" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="E76" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" t="n">
-        <v>192372.62</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0</v>
-      </c>
-      <c r="H76" t="n">
-        <v>0</v>
-      </c>
-      <c r="I76" t="n">
-        <v>0</v>
-      </c>
-      <c r="J76" t="n">
-        <v>1</v>
-      </c>
-      <c r="K76" t="n">
-        <v>1</v>
-      </c>
-      <c r="L76" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n"/>
-      <c r="B77" s="1" t="n"/>
-      <c r="C77" s="1" t="n"/>
-      <c r="D77" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" t="n">
-        <v>210433.92</v>
-      </c>
-      <c r="G77" t="n">
-        <v>0</v>
-      </c>
-      <c r="H77" t="n">
-        <v>0</v>
-      </c>
-      <c r="I77" t="n">
-        <v>0</v>
-      </c>
-      <c r="J77" t="n">
-        <v>1</v>
-      </c>
-      <c r="K77" t="n">
-        <v>1</v>
-      </c>
-      <c r="L77" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="n"/>
-      <c r="C78" s="1" t="n"/>
-      <c r="D78" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="E78" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" t="n">
-        <v>229197.77</v>
-      </c>
-      <c r="G78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J78" t="n">
-        <v>1</v>
-      </c>
-      <c r="K78" t="n">
-        <v>1</v>
-      </c>
-      <c r="L78" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="n"/>
-      <c r="C79" s="1" t="n"/>
-      <c r="D79" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" t="n">
-        <v>241852.37</v>
-      </c>
-      <c r="G79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H79" t="n">
-        <v>0</v>
-      </c>
-      <c r="I79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L79" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n"/>
-      <c r="B80" s="1" t="n"/>
-      <c r="C80" s="1" t="n"/>
-      <c r="D80" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="E80" t="n">
-        <v>0</v>
-      </c>
-      <c r="F80" t="n">
-        <v>258504.39</v>
-      </c>
-      <c r="G80" t="n">
-        <v>0</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0</v>
-      </c>
-      <c r="I80" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" t="n">
-        <v>1</v>
-      </c>
-      <c r="K80" t="n">
-        <v>1</v>
-      </c>
-      <c r="L80" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n"/>
-      <c r="B81" s="1" t="n"/>
-      <c r="C81" s="1" t="n"/>
-      <c r="D81" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="E81" t="n">
-        <v>0</v>
-      </c>
-      <c r="F81" t="n">
-        <v>288231.01</v>
-      </c>
-      <c r="G81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0</v>
-      </c>
-      <c r="J81" t="n">
-        <v>1</v>
-      </c>
-      <c r="K81" t="n">
-        <v>1</v>
-      </c>
-      <c r="L81" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="n"/>
-      <c r="C82" s="1" t="n"/>
-      <c r="D82" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="E82" t="n">
-        <v>0</v>
-      </c>
-      <c r="F82" t="n">
-        <v>339865.58</v>
-      </c>
-      <c r="G82" t="n">
-        <v>0</v>
-      </c>
-      <c r="H82" t="n">
-        <v>0</v>
-      </c>
-      <c r="I82" t="n">
-        <v>0</v>
-      </c>
-      <c r="J82" t="n">
-        <v>1</v>
-      </c>
-      <c r="K82" t="n">
-        <v>1</v>
-      </c>
-      <c r="L82" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n"/>
-      <c r="B83" s="1" t="n"/>
-      <c r="C83" s="1" t="n"/>
-      <c r="D83" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="E83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F83" t="n">
-        <v>410468.85</v>
-      </c>
-      <c r="G83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I83" t="n">
-        <v>0</v>
-      </c>
-      <c r="J83" t="n">
-        <v>1</v>
-      </c>
-      <c r="K83" t="n">
-        <v>1</v>
-      </c>
-      <c r="L83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n"/>
-      <c r="B84" s="1" t="n"/>
-      <c r="C84" s="1" t="n"/>
-      <c r="D84" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="E84" t="n">
-        <v>0</v>
-      </c>
-      <c r="F84" t="n">
-        <v>499168.53</v>
-      </c>
-      <c r="G84" t="n">
-        <v>0</v>
-      </c>
-      <c r="H84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I84" t="n">
-        <v>0</v>
-      </c>
-      <c r="J84" t="n">
-        <v>1</v>
-      </c>
-      <c r="K84" t="n">
-        <v>1</v>
-      </c>
-      <c r="L84" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="n"/>
-      <c r="C85" s="1" t="n"/>
-      <c r="D85" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="E85" t="n">
-        <v>0</v>
-      </c>
-      <c r="F85" t="n">
-        <v>585639.23</v>
-      </c>
-      <c r="G85" t="n">
-        <v>0</v>
-      </c>
-      <c r="H85" t="n">
-        <v>0</v>
-      </c>
-      <c r="I85" t="n">
-        <v>0</v>
-      </c>
-      <c r="J85" t="n">
-        <v>1</v>
-      </c>
-      <c r="K85" t="n">
-        <v>1</v>
-      </c>
-      <c r="L85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A2:A43"/>
-    <mergeCell ref="A44:A85"/>
-    <mergeCell ref="B2:B43"/>
-    <mergeCell ref="B44:B85"/>
-    <mergeCell ref="C2:C25"/>
-    <mergeCell ref="C26:C43"/>
-    <mergeCell ref="C44:C67"/>
-    <mergeCell ref="C68:C85"/>
+    <mergeCell ref="A2:A36"/>
+    <mergeCell ref="A37:A74"/>
+    <mergeCell ref="B2:B36"/>
+    <mergeCell ref="B37:B74"/>
+    <mergeCell ref="C2:C17"/>
+    <mergeCell ref="C18:C36"/>
+    <mergeCell ref="C37:C55"/>
+    <mergeCell ref="C56:C74"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>